<commit_message>
Re-plotting and updated minDCF and actDCF
</commit_message>
<xml_diff>
--- a/report/GMM.xlsx
+++ b/report/GMM.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>GMM</t>
   </si>
@@ -42,52 +42,49 @@
     <t xml:space="preserve">Pi = 0.9</t>
   </si>
   <si>
-    <t xml:space="preserve">RAW - NO PCA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full-Cov 512 GAU</t>
-  </si>
-  <si>
-    <t>0.283</t>
-  </si>
-  <si>
-    <t>0.285</t>
+    <t xml:space="preserve">GAUSSIANIZED - NO PCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tied Full-Cov 8 GAU</t>
+  </si>
+  <si>
+    <t>0.287</t>
+  </si>
+  <si>
+    <t>0.289</t>
+  </si>
+  <si>
+    <t>33.3</t>
+  </si>
+  <si>
+    <t>0.849</t>
+  </si>
+  <si>
+    <t>1.0</t>
   </si>
   <si>
     <t>0.8956</t>
   </si>
   <si>
-    <t>0.914</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAUSSIANIZED - NO PCA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full-Cov 128 GAU</t>
-  </si>
-  <si>
-    <t>0.300</t>
-  </si>
-  <si>
-    <t>0.301</t>
-  </si>
-  <si>
-    <t>0.7684</t>
-  </si>
-  <si>
-    <t>0.880</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tied Full-Cov 128 GAU</t>
-  </si>
-  <si>
-    <t>0.288</t>
-  </si>
-  <si>
-    <t>0.7847</t>
-  </si>
-  <si>
-    <t>0.870</t>
+    <t xml:space="preserve">Full-Cov 4 GAU</t>
+  </si>
+  <si>
+    <t>0.291</t>
+  </si>
+  <si>
+    <t>0.294</t>
+  </si>
+  <si>
+    <t>33.1</t>
+  </si>
+  <si>
+    <t>0.8923</t>
+  </si>
+  <si>
+    <t>0.997</t>
+  </si>
+  <si>
+    <t>0.8662</t>
   </si>
   <si>
     <t xml:space="preserve">(TEST DATASET)</t>
@@ -152,16 +149,15 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -676,10 +672,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="21.421875"/>
-    <col customWidth="1" min="7" max="7" width="7.7109375"/>
-    <col customWidth="1" min="8" max="8" width="8.421875"/>
-    <col customWidth="1" min="10" max="10" width="7.00390625"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" width="21.421875"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" width="7.7109375"/>
+    <col bestFit="1" customWidth="1" min="8" max="8" width="8.421875"/>
+    <col bestFit="1" customWidth="1" min="10" max="10" width="7.00390625"/>
   </cols>
   <sheetData>
     <row r="3" ht="21">
@@ -718,10 +714,10 @@
         <v>4</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -731,7 +727,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="5"/>
@@ -743,141 +739,112 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" ht="14.25">
-      <c r="B10" s="8" t="s">
+    <row r="10" ht="14.25"/>
+    <row r="11" ht="14.25">
+      <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" ht="14.25">
-      <c r="B11" t="s">
+    <row r="12" ht="14.25">
+      <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="H11" s="6" t="s">
+      <c r="F12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I11">
+      <c r="H12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25"/>
+    <row r="15" ht="23.25">
+      <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25"/>
-    <row r="13" ht="14.25">
-      <c r="B13" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25">
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="9" t="s">
+      <c r="D15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="B18" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="H14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14" s="5"/>
-      <c r="K14" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25">
-      <c r="B15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" s="5"/>
-      <c r="K15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25"/>
-    <row r="17" ht="23.25">
-      <c r="B17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" ht="14.25">
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25">
-      <c r="B19" s="8" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="B20" s="6"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="B21" s="6"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="B22" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25">
-      <c r="B23" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="B24" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Improved report and translated
</commit_message>
<xml_diff>
--- a/report/GMM.xlsx
+++ b/report/GMM.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>GMM</t>
   </si>
@@ -105,6 +105,9 @@
     <t>17.6</t>
   </si>
   <si>
+    <t xml:space="preserve">Tied Full-Cov 8 GAU </t>
+  </si>
+  <si>
     <t>0.290</t>
   </si>
   <si>
@@ -112,6 +115,12 @@
   </si>
   <si>
     <t>13.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tied Full-Cov 8 GAU (balanced) </t>
+  </si>
+  <si>
+    <t>15.0</t>
   </si>
 </sst>
 </file>
@@ -698,12 +707,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="2" max="2" width="21.421875"/>
+    <col customWidth="1" min="2" max="2" width="27.421875"/>
     <col bestFit="1" customWidth="1" min="7" max="7" width="7.7109375"/>
     <col bestFit="1" customWidth="1" min="8" max="8" width="8.421875"/>
     <col bestFit="1" customWidth="1" min="10" max="10" width="7.00390625"/>
   </cols>
   <sheetData>
+    <row r="2" ht="14.25"/>
     <row r="3" ht="21">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
@@ -870,20 +880,31 @@
     </row>
     <row r="19" ht="14.25">
       <c r="B19" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="B20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
         <v>31</v>
       </c>
-      <c r="F19" t="s">
+      <c r="E20" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" ht="14.25">
-      <c r="B20" s="6"/>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="21" ht="14.25"/>
     <row r="22" ht="14.25">

</xml_diff>